<commit_message>
Atualização Desafio Aula 13
</commit_message>
<xml_diff>
--- a/Turma grupos.xlsx
+++ b/Turma grupos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roberto.freixeira\Desktop\CursoAndroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFDC8AC-E9E3-4C72-A864-DA3945A91B61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF09DA7F-59E4-4CEF-82E0-8F0F15B24145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="0" windowWidth="15345" windowHeight="15600" xr2:uid="{837B43B3-A4D6-4E5D-B7F5-DFCB0D1B5176}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="15345" windowHeight="15600" xr2:uid="{837B43B3-A4D6-4E5D-B7F5-DFCB0D1B5176}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Marcos Renann Fernandes da Silva</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Thais  Brasil Lenhard</t>
   </si>
   <si>
-    <t>Jônatas pereira Cabral de Araujo</t>
-  </si>
-  <si>
     <t>Mariana Oliveira Campos Machado</t>
   </si>
   <si>
@@ -135,6 +132,24 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Leandro Freire da Silva</t>
+  </si>
+  <si>
+    <t>Jonatas Pereira Cabral de Araujo</t>
+  </si>
+  <si>
+    <t>Ronaldo da Costa Tavares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrícia Pedrosa Alves Braga </t>
+  </si>
+  <si>
+    <t>Lídice F do Carmo dos Santos</t>
+  </si>
+  <si>
+    <t>Julia Valerio Andrade</t>
   </si>
 </sst>
 </file>
@@ -489,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A42400-5E75-401D-B528-BAD929E69805}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,17 +518,17 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +536,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +546,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -541,143 +556,168 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A33">
-    <sortCondition ref="A3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:A66">
+    <sortCondition ref="A41"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Primeira aula de AndroidStudio
</commit_message>
<xml_diff>
--- a/Turma grupos.xlsx
+++ b/Turma grupos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roberto.freixeira\Desktop\CursoAndroid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF09DA7F-59E4-4CEF-82E0-8F0F15B24145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAC4187-0E2B-40D0-BAB7-B51A2FE08BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="600" windowWidth="15345" windowHeight="15600" xr2:uid="{837B43B3-A4D6-4E5D-B7F5-DFCB0D1B5176}"/>
+    <workbookView xWindow="11340" yWindow="195" windowWidth="15345" windowHeight="15600" xr2:uid="{837B43B3-A4D6-4E5D-B7F5-DFCB0D1B5176}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Marcos Renann Fernandes da Silva</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Julia Valerio Andrade</t>
+  </si>
+  <si>
+    <t>Aula 14</t>
+  </si>
+  <si>
+    <t>Grupo 5</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -504,34 +513,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A42400-5E75-401D-B528-BAD929E69805}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="2" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -539,127 +554,133 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -667,20 +688,23 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -716,8 +740,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:A66">
-    <sortCondition ref="A41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A49:A75">
+    <sortCondition ref="A49"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>